<commit_message>
Updated SO Header TCs
</commit_message>
<xml_diff>
--- a/templates/QARSF/SalesOrder_BaseData.xlsx
+++ b/templates/QARSF/SalesOrder_BaseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF728B01-F165-4882-9F65-24C39CE7BF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308BB722-E44B-4497-8AF8-0209486F80D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8757A3A6-C01C-441B-AD80-F1D095B81FF6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Customer</t>
   </si>
@@ -68,13 +68,49 @@
   </si>
   <si>
     <t>Automation5501-5 (Misc)</t>
+  </si>
+  <si>
+    <t>Inventory Division</t>
+  </si>
+  <si>
+    <t>Sales Division</t>
+  </si>
+  <si>
+    <t>Manufacturing User</t>
+  </si>
+  <si>
+    <t>Line Number</t>
+  </si>
+  <si>
+    <t>Record Processed</t>
+  </si>
+  <si>
+    <t>a7O410000004Nwj</t>
+  </si>
+  <si>
+    <t>a5B41000000PRNX</t>
+  </si>
+  <si>
+    <t>a811K000000k9cL</t>
+  </si>
+  <si>
+    <t>a6J1K000000Qgsa</t>
+  </si>
+  <si>
+    <t>a6J1K000000Qgsf</t>
+  </si>
+  <si>
+    <t>a6J1K000000Qgsk</t>
+  </si>
+  <si>
+    <t>a6J1K000000Qgsp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +122,19 @@
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF4A4A56"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -110,9 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +481,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,10 +506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03899CEA-C02A-4C36-B5F4-142E568CFB2D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,9 +519,10 @@
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -483,8 +535,29 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -497,8 +570,29 @@
       <c r="D2">
         <v>20</v>
       </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -508,8 +602,29 @@
       <c r="C3">
         <v>500</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -522,8 +637,29 @@
       <c r="D4">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -533,8 +669,29 @@
       <c r="C5">
         <v>20</v>
       </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>